<commit_message>
Continued processing and EDA
</commit_message>
<xml_diff>
--- a/Column_dictionary.xlsx
+++ b/Column_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catri\OneDrive\Documents\MSc HDA\Machine Learning\Machine-Learning-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{10C80D77-10C3-4BBB-BC61-8FB1C6096E5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1DE4D17B-CBDF-49A0-ABD0-11D4E09B1B42}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{10C80D77-10C3-4BBB-BC61-8FB1C6096E5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A28676A5-6AD8-48DF-A166-19455F55B355}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{71E77F43-4AF3-4810-96E5-5F07733E2AD2}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>WTGAIN</t>
   </si>
   <si>
-    <t xml:space="preserve">infant_sex </t>
-  </si>
-  <si>
     <t>weight_gain</t>
   </si>
   <si>
@@ -215,30 +212,15 @@
     <t>res_status</t>
   </si>
   <si>
-    <t>prior_other_terminations</t>
-  </si>
-  <si>
-    <t>prior_births_now_living</t>
-  </si>
-  <si>
-    <t>prior_births_now_dead</t>
-  </si>
-  <si>
     <t>num_prenatal_visits</t>
   </si>
   <si>
-    <t xml:space="preserve">payment_source </t>
-  </si>
-  <si>
     <t>m_height_in</t>
   </si>
   <si>
     <t>m_transferred</t>
   </si>
   <si>
-    <t>m_hispanic_origin</t>
-  </si>
-  <si>
     <t>admit_icu</t>
   </si>
   <si>
@@ -254,9 +236,6 @@
     <t>sex_imp</t>
   </si>
   <si>
-    <t>f_hispanic_origin</t>
-  </si>
-  <si>
     <t>f_education</t>
   </si>
   <si>
@@ -284,9 +263,6 @@
     <t>birth_place</t>
   </si>
   <si>
-    <t>no_riskf_reported</t>
-  </si>
-  <si>
     <t>gonorrhea</t>
   </si>
   <si>
@@ -305,36 +281,9 @@
     <t>marital_stat</t>
   </si>
   <si>
-    <t>no_m_morbidity_reported</t>
-  </si>
-  <si>
-    <t>prepregnancy_weight_r</t>
-  </si>
-  <si>
-    <t>delivery_method_r</t>
-  </si>
-  <si>
     <t>payment_r</t>
   </si>
   <si>
-    <t>m_race_r6</t>
-  </si>
-  <si>
-    <t>m_race_r15</t>
-  </si>
-  <si>
-    <t>m_race_r31</t>
-  </si>
-  <si>
-    <t>f_race_r6</t>
-  </si>
-  <si>
-    <t>f_race_r31</t>
-  </si>
-  <si>
-    <t>f_race_r15</t>
-  </si>
-  <si>
     <t>last_norm_menses_mn</t>
   </si>
   <si>
@@ -362,7 +311,58 @@
     <t>m_race_imp</t>
   </si>
   <si>
-    <t>no_infec_reported</t>
+    <t>prior_births_dead</t>
+  </si>
+  <si>
+    <t>prior_births_living</t>
+  </si>
+  <si>
+    <t>prior_terminations</t>
+  </si>
+  <si>
+    <t>prepreg_weight</t>
+  </si>
+  <si>
+    <t>delivery_method</t>
+  </si>
+  <si>
+    <t>infant_sex</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>infections</t>
+  </si>
+  <si>
+    <t>m_race15</t>
+  </si>
+  <si>
+    <t>m_race31</t>
+  </si>
+  <si>
+    <t>m_race6</t>
+  </si>
+  <si>
+    <t>f_race15</t>
+  </si>
+  <si>
+    <t>f_race31</t>
+  </si>
+  <si>
+    <t>f_race6</t>
+  </si>
+  <si>
+    <t>m_hispanic</t>
+  </si>
+  <si>
+    <t>f_hispanic</t>
+  </si>
+  <si>
+    <t>m_morbidity</t>
+  </si>
+  <si>
+    <t>riskf</t>
   </si>
 </sst>
 </file>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A195FC0-2E40-4538-9CD7-56EBDDC3557C}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -764,7 +764,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -780,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28">
@@ -788,7 +788,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28">
@@ -796,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -804,7 +804,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -812,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -820,7 +820,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -828,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -836,7 +836,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -844,7 +844,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28">
@@ -852,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -860,7 +860,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -868,7 +868,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -876,7 +876,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -884,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -892,7 +892,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -900,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -908,7 +908,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -916,7 +916,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -924,7 +924,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -932,7 +932,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -940,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -948,7 +948,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="28">
@@ -956,7 +956,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -964,7 +964,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="28">
@@ -972,7 +972,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -980,7 +980,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -988,7 +988,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -996,7 +996,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1004,7 +1004,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1012,7 +1012,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="28">
@@ -1020,7 +1020,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1028,7 +1028,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1036,7 +1036,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1044,7 +1044,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1052,7 +1052,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="28">
@@ -1060,7 +1060,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1068,7 +1068,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="28">
@@ -1092,7 +1092,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="28">
@@ -1108,15 +1108,15 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="28">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="28">
@@ -1124,15 +1124,15 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="28">
@@ -1140,7 +1140,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="28">
@@ -1148,7 +1148,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="28">
@@ -1164,7 +1164,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1172,7 +1172,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1180,7 +1180,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on processing and first models
</commit_message>
<xml_diff>
--- a/Column_dictionary.xlsx
+++ b/Column_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catri\OneDrive\Documents\MSc HDA\Machine Learning\Machine-Learning-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{10C80D77-10C3-4BBB-BC61-8FB1C6096E5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A28676A5-6AD8-48DF-A166-19455F55B355}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{10C80D77-10C3-4BBB-BC61-8FB1C6096E5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{193962D8-89DB-4FD0-8916-B4666D08A9B5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{71E77F43-4AF3-4810-96E5-5F07733E2AD2}"/>
   </bookViews>
@@ -239,9 +239,6 @@
     <t>f_education</t>
   </si>
   <si>
-    <t>f_combined_age</t>
-  </si>
-  <si>
     <t>birth_yr</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>marital_stat</t>
   </si>
   <si>
-    <t>payment_r</t>
-  </si>
-  <si>
     <t>last_norm_menses_mn</t>
   </si>
   <si>
@@ -363,6 +357,12 @@
   </si>
   <si>
     <t>riskf</t>
+  </si>
+  <si>
+    <t>payment_det</t>
+  </si>
+  <si>
+    <t>f_age</t>
   </si>
 </sst>
 </file>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A195FC0-2E40-4538-9CD7-56EBDDC3557C}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -764,7 +764,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -780,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28">
@@ -788,7 +788,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28">
@@ -796,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -804,7 +804,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -812,7 +812,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -820,7 +820,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -828,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -836,7 +836,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -844,7 +844,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28">
@@ -852,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -868,7 +868,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -876,7 +876,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -884,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -892,7 +892,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -900,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -908,7 +908,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -916,7 +916,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -932,7 +932,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -940,7 +940,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -948,7 +948,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="28">
@@ -964,7 +964,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="28">
@@ -988,7 +988,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1004,7 +1004,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1012,7 +1012,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="28">
@@ -1020,7 +1020,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1028,7 +1028,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1052,7 +1052,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="28">
@@ -1060,7 +1060,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1068,7 +1068,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="28">
@@ -1092,7 +1092,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1108,7 +1108,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="28">
@@ -1124,7 +1124,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1132,7 +1132,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="28">
@@ -1140,7 +1140,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="28">
@@ -1172,7 +1172,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:2">

</xml_diff>